<commit_message>
Classification Training and Prediction: Data Preparation and Model Input Architecture
</commit_message>
<xml_diff>
--- a/01_RawData/01_ClassificationTraining_DataPreparation.xlsx
+++ b/01_RawData/01_ClassificationTraining_DataPreparation.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Workspace\Branches\WEFN\01_RawData\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{022993DC-4C59-4335-B006-BC021297CA2A}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F5E1F2E5-4A04-4470-B481-A387527CC673}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-28920" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Data" sheetId="1" r:id="rId1"/>
@@ -182,22 +182,6 @@
     <phoneticPr fontId="19" type="noConversion"/>
   </si>
   <si>
-    <t>Active Working Population in Agriculture Percentage</t>
-    <phoneticPr fontId="19" type="noConversion"/>
-  </si>
-  <si>
-    <t>Yearly Population Increase Percentage</t>
-    <phoneticPr fontId="19" type="noConversion"/>
-  </si>
-  <si>
-    <t>Agricultural Products Import Value</t>
-    <phoneticPr fontId="19" type="noConversion"/>
-  </si>
-  <si>
-    <t>Agricultural Products Export Value</t>
-    <phoneticPr fontId="19" type="noConversion"/>
-  </si>
-  <si>
     <t>Population</t>
     <phoneticPr fontId="19" type="noConversion"/>
   </si>
@@ -250,11 +234,27 @@
     <phoneticPr fontId="19" type="noConversion"/>
   </si>
   <si>
-    <t>F3=(F3.1-F3.2)</t>
+    <t>F3=(F3.1-F3.2)/F3.3</t>
     <phoneticPr fontId="19" type="noConversion"/>
   </si>
   <si>
-    <t>Agricultural Products Net Import Value (Import-Export)</t>
+    <t>Agricultural Products Import Value (1000 USD)</t>
+    <phoneticPr fontId="19" type="noConversion"/>
+  </si>
+  <si>
+    <t>Agricultural Products Export Value (1000 USD)</t>
+    <phoneticPr fontId="19" type="noConversion"/>
+  </si>
+  <si>
+    <t>Agricultural Products Net Import Value (Import-Export) per Capita</t>
+    <phoneticPr fontId="19" type="noConversion"/>
+  </si>
+  <si>
+    <t>Yearly Population Increase Percentage (%)</t>
+    <phoneticPr fontId="19" type="noConversion"/>
+  </si>
+  <si>
+    <t>Active Working Population in Agriculture Percentage (%)</t>
     <phoneticPr fontId="19" type="noConversion"/>
   </si>
 </sst>
@@ -262,10 +262,11 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <numFmts count="1">
+  <numFmts count="2">
     <numFmt numFmtId="176" formatCode="0.0000"/>
+    <numFmt numFmtId="177" formatCode="0.000"/>
   </numFmts>
-  <fonts count="25" x14ac:knownFonts="1">
+  <fonts count="24">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -453,16 +454,6 @@
     </font>
     <font>
       <sz val="12"/>
-      <color theme="5" tint="-0.249977111117893"/>
-      <name val="新細明體"/>
-      <family val="1"/>
-      <charset val="136"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <u/>
-      <sz val="12"/>
-      <color theme="5" tint="-0.249977111117893"/>
       <name val="新細明體"/>
       <family val="1"/>
       <charset val="136"/>
@@ -471,7 +462,6 @@
     <font>
       <b/>
       <sz val="12"/>
-      <color theme="5" tint="-0.249977111117893"/>
       <name val="新細明體"/>
       <family val="1"/>
       <charset val="136"/>
@@ -906,7 +896,7 @@
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="11">
+  <cellXfs count="10">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
       <alignment vertical="center"/>
     </xf>
@@ -928,16 +918,13 @@
     <xf numFmtId="2" fontId="14" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="1" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1">
-      <alignment vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="22" fillId="0" borderId="0" xfId="0" applyFont="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="23" fillId="0" borderId="0" xfId="42" applyFont="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="24" fillId="0" borderId="0" xfId="0" applyFont="1">
+    <xf numFmtId="0" fontId="23" fillId="0" borderId="0" xfId="0" applyFont="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="177" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1">
       <alignment vertical="center"/>
     </xf>
   </cellXfs>
@@ -1298,25 +1285,25 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:N37"/>
   <sheetViews>
-    <sheetView zoomScaleNormal="100" workbookViewId="0">
-      <pane xSplit="1" ySplit="1" topLeftCell="B2" activePane="bottomRight" state="frozen"/>
+    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+      <pane xSplit="1" ySplit="1" topLeftCell="B23" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="F4" sqref="F4"/>
+      <selection pane="bottomRight" activeCell="G2" sqref="G2:G37"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="16.2" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="16.2"/>
   <cols>
     <col min="1" max="1" width="27.6640625" bestFit="1" customWidth="1"/>
     <col min="2" max="5" width="10.33203125" customWidth="1"/>
-    <col min="6" max="6" width="11.6640625" style="8" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="11.6640625" style="7" bestFit="1" customWidth="1"/>
     <col min="7" max="7" width="10.33203125" customWidth="1"/>
     <col min="8" max="8" width="12.77734375" customWidth="1"/>
     <col min="9" max="12" width="8.77734375" customWidth="1"/>
     <col min="14" max="14" width="10.5546875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:12" s="1" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:12" s="1" customFormat="1">
       <c r="A1" s="1" t="s">
         <v>40</v>
       </c>
@@ -1332,7 +1319,7 @@
       <c r="E1" s="1" t="s">
         <v>43</v>
       </c>
-      <c r="F1" s="10" t="s">
+      <c r="F1" s="8" t="s">
         <v>44</v>
       </c>
       <c r="G1" s="1" t="s">
@@ -1354,7 +1341,7 @@
         <v>39</v>
       </c>
     </row>
-    <row r="2" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:12">
       <c r="A2" t="s">
         <v>7</v>
       </c>
@@ -1370,12 +1357,12 @@
       <c r="E2">
         <v>313585</v>
       </c>
-      <c r="F2" s="8">
+      <c r="F2" s="7">
         <v>37383887</v>
       </c>
-      <c r="G2" s="7">
-        <f>D2-E2</f>
-        <v>9720152</v>
+      <c r="G2" s="9">
+        <f>(D2-E2)/F2</f>
+        <v>0.26000913174170465</v>
       </c>
       <c r="H2" s="4">
         <v>1.95141520944077</v>
@@ -1393,7 +1380,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="3" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:12">
       <c r="A3" t="s">
         <v>11</v>
       </c>
@@ -1409,12 +1396,12 @@
       <c r="E3">
         <v>20965</v>
       </c>
-      <c r="F3" s="8">
+      <c r="F3" s="7">
         <v>25107931</v>
       </c>
-      <c r="G3" s="7">
-        <f t="shared" ref="G3:G37" si="0">D3-E3</f>
-        <v>3535047</v>
+      <c r="G3" s="9">
+        <f t="shared" ref="G3:G37" si="0">(D3-E3)/F3</f>
+        <v>0.14079403834589158</v>
       </c>
       <c r="H3" s="4">
         <v>3.5977743076249902</v>
@@ -1432,7 +1419,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="4" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:12">
       <c r="A4" t="s">
         <v>24</v>
       </c>
@@ -1448,12 +1435,12 @@
       <c r="E4">
         <v>293369</v>
       </c>
-      <c r="F4" s="8">
+      <c r="F4" s="7">
         <v>2884229</v>
       </c>
-      <c r="G4" s="7">
-        <f t="shared" si="0"/>
-        <v>507190</v>
+      <c r="G4" s="9">
+        <f t="shared" si="0"/>
+        <v>0.17584942111045967</v>
       </c>
       <c r="H4" s="4">
         <v>0.26701321436823899</v>
@@ -1471,7 +1458,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="5" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:12">
       <c r="A5" t="s">
         <v>0</v>
       </c>
@@ -1487,12 +1474,12 @@
       <c r="E5">
         <v>484257</v>
       </c>
-      <c r="F5" s="8">
+      <c r="F5" s="7">
         <v>16571246</v>
       </c>
-      <c r="G5" s="7">
-        <f t="shared" si="0"/>
-        <v>-18263</v>
+      <c r="G5" s="9">
+        <f t="shared" si="0"/>
+        <v>-1.1020897281954537E-3</v>
       </c>
       <c r="H5" s="4">
         <v>2.9973924775883001</v>
@@ -1510,7 +1497,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="6" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:12">
       <c r="A6" t="s">
         <v>12</v>
       </c>
@@ -1526,12 +1513,12 @@
       <c r="E6">
         <v>53705319</v>
       </c>
-      <c r="F6" s="8">
+      <c r="F6" s="7">
         <v>1350695000</v>
       </c>
-      <c r="G6" s="7">
-        <f t="shared" si="0"/>
-        <v>90931549</v>
+      <c r="G6" s="9">
+        <f t="shared" si="0"/>
+        <v>6.7322044577051071E-2</v>
       </c>
       <c r="H6" s="4">
         <v>0.487231117971201</v>
@@ -1549,7 +1536,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="7" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:12">
       <c r="A7" t="s">
         <v>27</v>
       </c>
@@ -1565,12 +1552,12 @@
       <c r="E7">
         <v>3838195</v>
       </c>
-      <c r="F7" s="8">
+      <c r="F7" s="7">
         <v>4688000</v>
       </c>
-      <c r="G7" s="7">
-        <f t="shared" si="0"/>
-        <v>-2116964</v>
+      <c r="G7" s="9">
+        <f t="shared" si="0"/>
+        <v>-0.45157081911262797</v>
       </c>
       <c r="H7" s="4">
         <v>1.1782883525971199</v>
@@ -1588,7 +1575,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="8" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:12">
       <c r="A8" t="s">
         <v>1</v>
       </c>
@@ -1604,12 +1591,12 @@
       <c r="E8">
         <v>2373603</v>
       </c>
-      <c r="F8" s="8">
+      <c r="F8" s="7">
         <v>92726971</v>
       </c>
-      <c r="G8" s="7">
-        <f t="shared" si="0"/>
-        <v>-895662</v>
+      <c r="G8" s="9">
+        <f t="shared" si="0"/>
+        <v>-9.6591314300560945E-3</v>
       </c>
       <c r="H8" s="4">
         <v>2.8296172142251699</v>
@@ -1627,7 +1614,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="9" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:12">
       <c r="A9" t="s">
         <v>2</v>
       </c>
@@ -1643,12 +1630,12 @@
       <c r="E9">
         <v>2699118</v>
       </c>
-      <c r="F9" s="8">
+      <c r="F9" s="7">
         <v>25996449</v>
       </c>
-      <c r="G9" s="7">
-        <f t="shared" si="0"/>
-        <v>-1143519</v>
+      <c r="G9" s="9">
+        <f t="shared" si="0"/>
+        <v>-4.3987507678452546E-2</v>
       </c>
       <c r="H9" s="4">
         <v>2.3694753111338902</v>
@@ -1666,7 +1653,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="10" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:12">
       <c r="A10" t="s">
         <v>14</v>
       </c>
@@ -1682,12 +1669,12 @@
       <c r="E10">
         <v>4782746</v>
       </c>
-      <c r="F10" s="8">
+      <c r="F10" s="7">
         <v>14781942</v>
       </c>
-      <c r="G10" s="7">
-        <f t="shared" si="0"/>
-        <v>-2482758</v>
+      <c r="G10" s="9">
+        <f t="shared" si="0"/>
+        <v>-0.16795885141478703</v>
       </c>
       <c r="H10" s="4">
         <v>1.77749578673149</v>
@@ -1705,7 +1692,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="11" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:12">
       <c r="A11" t="s">
         <v>28</v>
       </c>
@@ -1721,12 +1708,12 @@
       <c r="E11">
         <v>38166024</v>
       </c>
-      <c r="F11" s="8">
+      <c r="F11" s="7">
         <v>1265782790</v>
       </c>
-      <c r="G11" s="7">
-        <f t="shared" si="0"/>
-        <v>-17980589</v>
+      <c r="G11" s="9">
+        <f t="shared" si="0"/>
+        <v>-1.4205114133365646E-2</v>
       </c>
       <c r="H11" s="4">
         <v>1.2316229280211299</v>
@@ -1744,7 +1731,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="12" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:12">
       <c r="A12" t="s">
         <v>29</v>
       </c>
@@ -1760,12 +1747,12 @@
       <c r="E12">
         <v>38281998</v>
       </c>
-      <c r="F12" s="8">
+      <c r="F12" s="7">
         <v>248452413</v>
       </c>
-      <c r="G12" s="7">
-        <f t="shared" si="0"/>
-        <v>-20893102</v>
+      <c r="G12" s="9">
+        <f t="shared" si="0"/>
+        <v>-8.4092972765774668E-2</v>
       </c>
       <c r="H12" s="4">
         <v>1.35189219176242</v>
@@ -1783,7 +1770,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="13" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:12">
       <c r="A13" t="s">
         <v>23</v>
       </c>
@@ -1799,12 +1786,12 @@
       <c r="E13">
         <v>2362798</v>
       </c>
-      <c r="F13" s="8">
+      <c r="F13" s="7">
         <v>7910500</v>
       </c>
-      <c r="G13" s="7">
-        <f t="shared" si="0"/>
-        <v>2587374</v>
+      <c r="G13" s="9">
+        <f t="shared" si="0"/>
+        <v>0.32708096833322797</v>
       </c>
       <c r="H13" s="4">
         <v>1.8461513212671099</v>
@@ -1822,7 +1809,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="14" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:12">
       <c r="A14" t="s">
         <v>25</v>
       </c>
@@ -1838,12 +1825,12 @@
       <c r="E14">
         <v>40109043</v>
       </c>
-      <c r="F14" s="8">
+      <c r="F14" s="7">
         <v>59539717</v>
       </c>
-      <c r="G14" s="7">
-        <f t="shared" si="0"/>
-        <v>5047714</v>
+      <c r="G14" s="9">
+        <f t="shared" si="0"/>
+        <v>8.4778938401739459E-2</v>
       </c>
       <c r="H14" s="4">
         <v>0.26954123952099601</v>
@@ -1861,7 +1848,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="15" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:12">
       <c r="A15" t="s">
         <v>22</v>
       </c>
@@ -1877,12 +1864,12 @@
       <c r="E15">
         <v>368032</v>
       </c>
-      <c r="F15" s="8">
+      <c r="F15" s="7">
         <v>2842132</v>
       </c>
-      <c r="G15" s="7">
-        <f t="shared" si="0"/>
-        <v>622653</v>
+      <c r="G15" s="9">
+        <f t="shared" si="0"/>
+        <v>0.2190795501405283</v>
       </c>
       <c r="H15" s="4">
         <v>0.57173146642299799</v>
@@ -1900,7 +1887,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="16" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:12">
       <c r="A16" t="s">
         <v>18</v>
       </c>
@@ -1916,12 +1903,12 @@
       <c r="E16">
         <v>3287133</v>
       </c>
-      <c r="F16" s="8">
+      <c r="F16" s="7">
         <v>127629000</v>
       </c>
-      <c r="G16" s="7">
-        <f t="shared" si="0"/>
-        <v>63268603</v>
+      <c r="G16" s="9">
+        <f t="shared" si="0"/>
+        <v>0.49572278243972767</v>
       </c>
       <c r="H16" s="4">
         <v>-0.15971067584434701</v>
@@ -1939,7 +1926,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="17" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:14">
       <c r="A17" t="s">
         <v>21</v>
       </c>
@@ -1955,12 +1942,12 @@
       <c r="E17">
         <v>1370229</v>
       </c>
-      <c r="F17" s="8">
+      <c r="F17" s="7">
         <v>8090872</v>
       </c>
-      <c r="G17" s="7">
-        <f t="shared" si="0"/>
-        <v>2172943</v>
+      <c r="G17" s="9">
+        <f t="shared" si="0"/>
+        <v>0.26856721994860383</v>
       </c>
       <c r="H17" s="4">
         <v>5.4315865678996902</v>
@@ -1978,7 +1965,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="18" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:14">
       <c r="A18" t="s">
         <v>3</v>
       </c>
@@ -1994,12 +1981,12 @@
       <c r="E18">
         <v>2069926</v>
       </c>
-      <c r="F18" s="8">
+      <c r="F18" s="7">
         <v>44343410</v>
       </c>
-      <c r="G18" s="7">
-        <f t="shared" si="0"/>
-        <v>-398785</v>
+      <c r="G18" s="9">
+        <f t="shared" si="0"/>
+        <v>-8.9931063037326179E-3</v>
       </c>
       <c r="H18" s="4">
         <v>2.6627048597740899</v>
@@ -2017,7 +2004,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="19" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="19" spans="1:14">
       <c r="A19" t="s">
         <v>41</v>
       </c>
@@ -2033,12 +2020,12 @@
       <c r="E19">
         <v>27287</v>
       </c>
-      <c r="F19" s="8">
+      <c r="F19" s="7">
         <v>24800612</v>
       </c>
-      <c r="G19" s="7">
-        <f t="shared" si="0"/>
-        <v>590089</v>
+      <c r="G19" s="9">
+        <f t="shared" si="0"/>
+        <v>2.3793324132485118E-2</v>
       </c>
       <c r="H19" s="4">
         <v>0.51431979694602203</v>
@@ -2056,7 +2043,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="20" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="20" spans="1:14">
       <c r="A20" t="s">
         <v>20</v>
       </c>
@@ -2072,12 +2059,12 @@
       <c r="E20">
         <v>5032328</v>
       </c>
-      <c r="F20" s="8">
+      <c r="F20" s="7">
         <v>50199853</v>
       </c>
-      <c r="G20" s="7">
-        <f t="shared" si="0"/>
-        <v>19817132</v>
+      <c r="G20" s="9">
+        <f t="shared" si="0"/>
+        <v>0.39476474164177333</v>
       </c>
       <c r="H20" s="4">
         <v>0.52571366060041402</v>
@@ -2095,9 +2082,9 @@
         <v>0</v>
       </c>
     </row>
-    <row r="21" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="21" spans="1:14">
       <c r="A21" t="s">
-        <v>61</v>
+        <v>57</v>
       </c>
       <c r="B21" s="5">
         <v>8726.2804965044907</v>
@@ -2111,12 +2098,12 @@
       <c r="E21">
         <v>263327</v>
       </c>
-      <c r="F21" s="8">
+      <c r="F21" s="7">
         <v>5607200</v>
       </c>
-      <c r="G21" s="7">
-        <f t="shared" si="0"/>
-        <v>505673</v>
+      <c r="G21" s="9">
+        <f t="shared" si="0"/>
+        <v>9.018280068483378E-2</v>
       </c>
       <c r="H21" s="4">
         <v>1.6652365593996199</v>
@@ -2134,7 +2121,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="22" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="22" spans="1:14">
       <c r="A22" t="s">
         <v>19</v>
       </c>
@@ -2150,12 +2137,12 @@
       <c r="E22">
         <v>614971</v>
       </c>
-      <c r="F22" s="8">
+      <c r="F22" s="7">
         <v>5538634</v>
       </c>
-      <c r="G22" s="7">
-        <f t="shared" si="0"/>
-        <v>2529879</v>
+      <c r="G22" s="9">
+        <f t="shared" si="0"/>
+        <v>0.45676948503909087</v>
       </c>
       <c r="H22" s="4">
         <v>6.26387989274438</v>
@@ -2173,7 +2160,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="23" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="23" spans="1:14">
       <c r="A23" t="s">
         <v>5</v>
       </c>
@@ -2189,12 +2176,12 @@
       <c r="E23">
         <v>3838</v>
       </c>
-      <c r="F23" s="8">
+      <c r="F23" s="7">
         <v>2014990</v>
       </c>
-      <c r="G23" s="7">
-        <f t="shared" si="0"/>
-        <v>216084</v>
+      <c r="G23" s="9">
+        <f t="shared" si="0"/>
+        <v>0.10723824932133658</v>
       </c>
       <c r="H23" s="4">
         <v>0.557534245861524</v>
@@ -2212,7 +2199,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="24" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="24" spans="1:14">
       <c r="A24" t="s">
         <v>26</v>
       </c>
@@ -2228,12 +2215,12 @@
       <c r="E24">
         <v>30875352</v>
       </c>
-      <c r="F24" s="8">
+      <c r="F24" s="7">
         <v>29068159</v>
       </c>
-      <c r="G24" s="7">
-        <f t="shared" si="0"/>
-        <v>-11944556</v>
+      <c r="G24" s="9">
+        <f t="shared" si="0"/>
+        <v>-0.41091546251690725</v>
       </c>
       <c r="H24" s="4">
         <v>1.44566067334625</v>
@@ -2251,7 +2238,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="25" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="25" spans="1:14">
       <c r="A25" t="s">
         <v>30</v>
       </c>
@@ -2267,12 +2254,12 @@
       <c r="E25">
         <v>21656035</v>
       </c>
-      <c r="F25" s="8">
+      <c r="F25" s="7">
         <v>117274155</v>
       </c>
-      <c r="G25" s="7">
-        <f t="shared" si="0"/>
-        <v>4993315</v>
+      <c r="G25" s="9">
+        <f t="shared" si="0"/>
+        <v>4.2578136674700409E-2</v>
       </c>
       <c r="H25" s="4">
         <v>1.3552892520419</v>
@@ -2290,7 +2277,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="26" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="26" spans="1:14">
       <c r="A26" t="s">
         <v>31</v>
       </c>
@@ -2307,12 +2294,12 @@
       <c r="E26">
         <v>81900</v>
       </c>
-      <c r="F26" s="8">
+      <c r="F26" s="7">
         <v>620601</v>
       </c>
-      <c r="G26" s="7">
-        <f t="shared" si="0"/>
-        <v>476316</v>
+      <c r="G26" s="9">
+        <f t="shared" si="0"/>
+        <v>0.76750762567253361</v>
       </c>
       <c r="H26" s="4">
         <v>8.4147408002309396E-2</v>
@@ -2331,7 +2318,7 @@
       </c>
       <c r="N26" s="6"/>
     </row>
-    <row r="27" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="27" spans="1:14">
       <c r="A27" t="s">
         <v>6</v>
       </c>
@@ -2347,12 +2334,12 @@
       <c r="E27">
         <v>2101379</v>
       </c>
-      <c r="F27" s="8">
+      <c r="F27" s="7">
         <v>33241898</v>
       </c>
-      <c r="G27" s="7">
-        <f t="shared" si="0"/>
-        <v>3632644</v>
+      <c r="G27" s="9">
+        <f t="shared" si="0"/>
+        <v>0.1092790790706355</v>
       </c>
       <c r="H27" s="4">
         <v>1.3936059661850999</v>
@@ -2370,7 +2357,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="28" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="28" spans="1:14">
       <c r="A28" t="s">
         <v>10</v>
       </c>
@@ -2386,12 +2373,12 @@
       <c r="E28">
         <v>237990</v>
       </c>
-      <c r="F28" s="8">
+      <c r="F28" s="7">
         <v>26989862</v>
       </c>
-      <c r="G28" s="7">
-        <f t="shared" si="0"/>
-        <v>682269</v>
+      <c r="G28" s="9">
+        <f t="shared" si="0"/>
+        <v>2.5278713911171535E-2</v>
       </c>
       <c r="H28" s="4">
         <v>-0.19090792417970401</v>
@@ -2409,7 +2396,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="29" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="29" spans="1:14">
       <c r="A29" t="s">
         <v>4</v>
       </c>
@@ -2425,12 +2412,12 @@
       <c r="E29">
         <v>4712503</v>
       </c>
-      <c r="F29" s="8">
+      <c r="F29" s="7">
         <v>187281475</v>
       </c>
-      <c r="G29" s="7">
-        <f t="shared" si="0"/>
-        <v>1020349</v>
+      <c r="G29" s="9">
+        <f t="shared" si="0"/>
+        <v>5.4482110416953942E-3</v>
       </c>
       <c r="H29" s="4">
         <v>2.1267117557463999</v>
@@ -2448,7 +2435,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="30" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="30" spans="1:14">
       <c r="A30" t="s">
         <v>16</v>
       </c>
@@ -2464,12 +2451,12 @@
       <c r="E30">
         <v>4203359</v>
       </c>
-      <c r="F30" s="8">
+      <c r="F30" s="7">
         <v>29506788</v>
       </c>
-      <c r="G30" s="7">
-        <f t="shared" si="0"/>
-        <v>146411</v>
+      <c r="G30" s="9">
+        <f t="shared" si="0"/>
+        <v>4.9619429942696575E-3</v>
       </c>
       <c r="H30" s="4">
         <v>0.82513803881188197</v>
@@ -2487,7 +2474,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="31" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="31" spans="1:14">
       <c r="A31" t="s">
         <v>17</v>
       </c>
@@ -2503,12 +2490,12 @@
       <c r="E31">
         <v>8463777</v>
       </c>
-      <c r="F31" s="8">
+      <c r="F31" s="7">
         <v>5312437</v>
       </c>
-      <c r="G31" s="7">
-        <f t="shared" si="0"/>
-        <v>3125712</v>
+      <c r="G31" s="9">
+        <f t="shared" si="0"/>
+        <v>0.58837629509771128</v>
       </c>
       <c r="H31" s="4">
         <v>2.4533903303101798</v>
@@ -2526,7 +2513,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="32" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="32" spans="1:14">
       <c r="A32" t="s">
         <v>9</v>
       </c>
@@ -2542,12 +2529,12 @@
       <c r="E32">
         <v>638248</v>
       </c>
-      <c r="F32" s="8">
+      <c r="F32" s="7">
         <v>20442541</v>
       </c>
-      <c r="G32" s="7">
-        <f t="shared" si="0"/>
-        <v>1783367</v>
+      <c r="G32" s="9">
+        <f t="shared" si="0"/>
+        <v>8.7238029753737567E-2</v>
       </c>
       <c r="H32" s="4">
         <v>-3.0847343185318801</v>
@@ -2565,7 +2552,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="33" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="33" spans="1:12">
       <c r="A33" t="s">
         <v>15</v>
       </c>
@@ -2581,12 +2568,12 @@
       <c r="E33">
         <v>141893</v>
       </c>
-      <c r="F33" s="8">
+      <c r="F33" s="7">
         <v>7874835</v>
       </c>
-      <c r="G33" s="7">
-        <f t="shared" si="0"/>
-        <v>479280</v>
+      <c r="G33" s="9">
+        <f t="shared" si="0"/>
+        <v>6.086222758953045E-2</v>
       </c>
       <c r="H33" s="4">
         <v>2.2775332172473699</v>
@@ -2604,9 +2591,9 @@
         <v>0</v>
       </c>
     </row>
-    <row r="34" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="34" spans="1:12">
       <c r="A34" t="s">
-        <v>62</v>
+        <v>58</v>
       </c>
       <c r="B34" s="5">
         <v>1785.2406124982001</v>
@@ -2620,12 +2607,12 @@
       <c r="E34">
         <v>1587723</v>
       </c>
-      <c r="F34" s="8">
+      <c r="F34" s="7">
         <v>47052481</v>
       </c>
-      <c r="G34" s="7">
-        <f t="shared" si="0"/>
-        <v>-289693</v>
+      <c r="G34" s="9">
+        <f t="shared" si="0"/>
+        <v>-6.1568060566243041E-3</v>
       </c>
       <c r="H34" s="4">
         <v>2.9748881696736298</v>
@@ -2643,7 +2630,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="35" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="35" spans="1:12">
       <c r="A35" t="s">
         <v>13</v>
       </c>
@@ -2659,12 +2646,12 @@
       <c r="E35">
         <v>32640301</v>
       </c>
-      <c r="F35" s="8">
+      <c r="F35" s="7">
         <v>67835957</v>
       </c>
-      <c r="G35" s="7">
-        <f t="shared" si="0"/>
-        <v>-21735556</v>
+      <c r="G35" s="9">
+        <f t="shared" si="0"/>
+        <v>-0.32041349398225488</v>
       </c>
       <c r="H35" s="4">
         <v>0.469250686880267</v>
@@ -2682,7 +2669,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="36" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="36" spans="1:12">
       <c r="A36" t="s">
         <v>8</v>
       </c>
@@ -2698,12 +2685,12 @@
       <c r="E36">
         <v>1476032</v>
       </c>
-      <c r="F36" s="8">
+      <c r="F36" s="7">
         <v>10847002</v>
       </c>
-      <c r="G36" s="7">
-        <f t="shared" si="0"/>
-        <v>1183359</v>
+      <c r="G36" s="9">
+        <f t="shared" si="0"/>
+        <v>0.10909549016401029</v>
       </c>
       <c r="H36" s="4">
         <v>0.97386081240491396</v>
@@ -2721,9 +2708,9 @@
         <v>0</v>
       </c>
     </row>
-    <row r="37" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="37" spans="1:12">
       <c r="A37" t="s">
-        <v>63</v>
+        <v>59</v>
       </c>
       <c r="B37" s="5">
         <v>2276.2874505211598</v>
@@ -2737,12 +2724,12 @@
       <c r="E37">
         <v>28644375</v>
       </c>
-      <c r="F37" s="8">
+      <c r="F37" s="7">
         <v>63700215</v>
       </c>
-      <c r="G37" s="7">
-        <f t="shared" si="0"/>
-        <v>31502366</v>
+      <c r="G37" s="9">
+        <f t="shared" si="0"/>
+        <v>0.49454096818982479</v>
       </c>
       <c r="H37" s="4">
         <v>0.69535313232226903</v>
@@ -2775,17 +2762,17 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{78054FFB-0FC1-404F-8536-4A80A54A69F6}">
   <dimension ref="A1:D9"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
-      <selection activeCell="D18" sqref="D18"/>
+    <sheetView zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
+      <selection activeCell="B16" sqref="B16"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="16.2" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="16.2"/>
   <cols>
     <col min="2" max="2" width="63.77734375" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="70.109375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" s="1" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:4" s="1" customFormat="1">
       <c r="A1" s="1" t="s">
         <v>46</v>
       </c>
@@ -2799,116 +2786,116 @@
         <v>47</v>
       </c>
     </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:4">
       <c r="A2" s="2" t="s">
         <v>32</v>
       </c>
       <c r="B2" t="s">
-        <v>55</v>
+        <v>51</v>
       </c>
       <c r="C2">
         <v>2012</v>
       </c>
       <c r="D2" s="3" t="s">
-        <v>54</v>
-      </c>
-    </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.3">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="3" spans="1:4">
       <c r="A3" s="2" t="s">
-        <v>65</v>
+        <v>61</v>
       </c>
       <c r="B3" t="s">
-        <v>56</v>
+        <v>52</v>
       </c>
       <c r="C3">
         <v>2003</v>
       </c>
       <c r="D3" s="3" t="s">
-        <v>57</v>
-      </c>
-    </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.3">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="4" spans="1:4">
       <c r="A4" s="2" t="s">
         <v>33</v>
       </c>
       <c r="B4" t="s">
-        <v>49</v>
+        <v>67</v>
       </c>
       <c r="C4">
         <v>2012</v>
       </c>
       <c r="D4" s="3" t="s">
-        <v>58</v>
-      </c>
-    </row>
-    <row r="5" spans="1:4" x14ac:dyDescent="0.3">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="5" spans="1:4">
       <c r="A5" s="2" t="s">
-        <v>42</v>
+        <v>34</v>
       </c>
       <c r="B5" t="s">
-        <v>51</v>
+        <v>65</v>
       </c>
       <c r="C5">
         <v>2012</v>
       </c>
-      <c r="D5" s="3" t="s">
-        <v>59</v>
-      </c>
-    </row>
-    <row r="6" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="D5" t="s">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="6" spans="1:4">
       <c r="A6" s="2" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="B6" t="s">
-        <v>52</v>
+        <v>63</v>
       </c>
       <c r="C6">
         <v>2012</v>
       </c>
       <c r="D6" s="3" t="s">
-        <v>59</v>
-      </c>
-    </row>
-    <row r="7" spans="1:4" s="8" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A7" s="8" t="s">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="7" spans="1:4">
+      <c r="A7" s="2" t="s">
+        <v>43</v>
+      </c>
+      <c r="B7" t="s">
+        <v>64</v>
+      </c>
+      <c r="C7">
+        <v>2012</v>
+      </c>
+      <c r="D7" s="3" t="s">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="8" spans="1:4" s="7" customFormat="1">
+      <c r="A8" s="7" t="s">
         <v>44</v>
       </c>
-      <c r="B7" s="8" t="s">
-        <v>53</v>
-      </c>
-      <c r="C7" s="8">
+      <c r="B8" s="7" t="s">
+        <v>49</v>
+      </c>
+      <c r="C8" s="7">
         <v>2012</v>
       </c>
-      <c r="D7" s="9" t="s">
-        <v>60</v>
-      </c>
-    </row>
-    <row r="8" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A8" s="2" t="s">
-        <v>34</v>
-      </c>
-      <c r="B8" t="s">
-        <v>67</v>
-      </c>
-      <c r="C8">
-        <v>2012</v>
-      </c>
-      <c r="D8" t="s">
-        <v>66</v>
-      </c>
-    </row>
-    <row r="9" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="D8" s="3" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="9" spans="1:4">
       <c r="A9" s="2" t="s">
         <v>35</v>
       </c>
       <c r="B9" t="s">
-        <v>50</v>
+        <v>66</v>
       </c>
       <c r="C9">
         <v>2012</v>
       </c>
       <c r="D9" s="3" t="s">
-        <v>64</v>
+        <v>60</v>
       </c>
     </row>
   </sheetData>
@@ -2917,9 +2904,9 @@
     <hyperlink ref="D2" r:id="rId1" xr:uid="{A7146BE5-EF42-42A1-AC31-27F10D420D1C}"/>
     <hyperlink ref="D3" r:id="rId2" xr:uid="{0E32973A-DED0-45A3-9388-05F2F1472BBF}"/>
     <hyperlink ref="D4" r:id="rId3" xr:uid="{F6364954-13BD-4B3C-99CB-B9E03833ABB1}"/>
-    <hyperlink ref="D5" r:id="rId4" location="data/TP" xr:uid="{A9353E61-3827-4843-99EE-7692F3174CDB}"/>
-    <hyperlink ref="D6" r:id="rId5" location="data/TP" xr:uid="{CC854199-35F0-46AB-A21B-469A2039C19C}"/>
-    <hyperlink ref="D7" r:id="rId6" xr:uid="{5974CCD7-22A7-4112-8685-063FF9C35436}"/>
+    <hyperlink ref="D6" r:id="rId4" location="data/TP" xr:uid="{A9353E61-3827-4843-99EE-7692F3174CDB}"/>
+    <hyperlink ref="D7" r:id="rId5" location="data/TP" xr:uid="{CC854199-35F0-46AB-A21B-469A2039C19C}"/>
+    <hyperlink ref="D8" r:id="rId6" xr:uid="{5974CCD7-22A7-4112-8685-063FF9C35436}"/>
     <hyperlink ref="D9" r:id="rId7" xr:uid="{88B952DC-725A-49B1-A1D9-0DAF40796F37}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>